<commit_message>
corrected xpaths for changed objects; added viewport for chrome headless
</commit_message>
<xml_diff>
--- a/OutputFiles/TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx
+++ b/OutputFiles/TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx
@@ -8,12 +8,15 @@
   <sheets>
     <sheet name="CypherOutput" r:id="rId3" sheetId="1"/>
     <sheet name="Message" r:id="rId4" sheetId="2"/>
+    <sheet name="CypherOutput_Message" r:id="rId5" sheetId="3"/>
+    <sheet name="StatOutput" r:id="rId6" sheetId="4"/>
+    <sheet name="StatOutput_Message" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="50">
   <si>
     <t>Case ID</t>
   </si>
@@ -139,6 +142,30 @@
   </si>
   <si>
     <t>C:\Users\radhakrishnang2\Desktop\Commons_Automation\OutputFiles\TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>Cypher query should not be an empty string</t>
+  </si>
+  <si>
+    <t>number_of_files</t>
+  </si>
+  <si>
+    <t>number_of_sample</t>
+  </si>
+  <si>
+    <t>number_of_cases</t>
+  </si>
+  <si>
+    <t>number_of_study</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
 </sst>
 </file>
@@ -173,10 +200,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -185,7 +212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
@@ -400,4 +427,226 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>